<commit_message>
Inicio do diagrama de gantt
</commit_message>
<xml_diff>
--- a/docs/docs_rodada1/Custo do Projeto.xlsx
+++ b/docs/docs_rodada1/Custo do Projeto.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26424"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A2F4F84DBF29CBDC3C989154D52528E350C23990" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70FE9937-A055-494A-A827-6015AD051C37}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_A2F4F84DBF29CBDC3C989154D52528E350C23990" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48BC7D14-DB6B-471A-9320-D655ABB9C16E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>numero</t>
   </si>
@@ -66,7 +66,7 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>Definição de Objetivos e Escopo do Projeto</t>
+    <t>Escopo do Produto e Projeto</t>
   </si>
   <si>
     <t>dias (expediente de 2h)</t>
@@ -75,22 +75,16 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>Criação do Documento de visão do Projeto</t>
+    <t>Identificação de Requisitos de Negócios e Técnicos</t>
   </si>
   <si>
     <t>1.3</t>
   </si>
   <si>
-    <t>Identificação de Requisitos de Negócios e Técnicos</t>
+    <t>Desenvolvimento do Plano de Projeto</t>
   </si>
   <si>
     <t>1.4</t>
-  </si>
-  <si>
-    <t>Desenvolvimento do Plano de Projeto</t>
-  </si>
-  <si>
-    <t>1.5</t>
   </si>
   <si>
     <t>Identificação dos Recursos necessários</t>
@@ -800,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -862,26 +856,26 @@
       </c>
       <c r="D3" s="11">
         <f>SUM(D4:D8)</f>
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F3" s="12">
         <f>SUM(D3,D10,D16,D27,D22,D32)</f>
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="G3" s="13">
         <f>F3/5</f>
-        <v>66.2</v>
+        <v>62.2</v>
       </c>
       <c r="I3" s="14">
         <v>31</v>
       </c>
       <c r="J3" s="15">
         <f>I3*F3</f>
-        <v>10261</v>
+        <v>9641</v>
       </c>
       <c r="K3" s="15">
         <f>J3+J3*L3</f>
-        <v>12313.2</v>
+        <v>11569.2</v>
       </c>
       <c r="L3" s="16">
         <v>0.2</v>
@@ -911,11 +905,11 @@
         <v>15</v>
       </c>
       <c r="D5" s="20">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G5" s="22">
         <f>G3/2</f>
-        <v>33.1</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="55.5" customHeight="1">
@@ -927,32 +921,26 @@
         <v>17</v>
       </c>
       <c r="D6" s="20">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="55.5" customHeight="1">
       <c r="A7" s="17"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="20">
-        <v>15</v>
+      <c r="D7" s="25">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="55.5" customHeight="1">
       <c r="A8" s="17"/>
-      <c r="B8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="25">
-        <v>10</v>
-      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1"/>
@@ -963,10 +951,10 @@
     <row r="10" spans="1:12" ht="27.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="11">
         <f>SUM(D11:D14)</f>
@@ -976,10 +964,10 @@
     <row r="11" spans="1:12" ht="58.5" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="20">
         <v>4</v>
@@ -988,10 +976,10 @@
     <row r="12" spans="1:12" ht="58.5" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="20">
         <v>4</v>
@@ -1000,10 +988,10 @@
     <row r="13" spans="1:12" ht="58.5" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D13" s="20">
         <v>3</v>
@@ -1012,10 +1000,10 @@
     <row r="14" spans="1:12" ht="58.5" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="25">
         <v>4</v>
@@ -1030,10 +1018,10 @@
     <row r="16" spans="1:12" ht="27.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="11">
         <f>SUM(D17:D20)</f>
@@ -1043,10 +1031,10 @@
     <row r="17" spans="1:4" ht="55.5" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="20">
         <v>8</v>
@@ -1055,10 +1043,10 @@
     <row r="18" spans="1:4" ht="55.5" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="20">
         <v>6</v>
@@ -1067,10 +1055,10 @@
     <row r="19" spans="1:4" ht="55.5" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="20">
         <v>16</v>
@@ -1079,10 +1067,10 @@
     <row r="20" spans="1:4" ht="55.5" customHeight="1">
       <c r="A20" s="17"/>
       <c r="B20" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="25">
         <v>8</v>
@@ -1097,10 +1085,10 @@
     <row r="22" spans="1:4" ht="27.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="11">
         <f>SUM(D23:D25)</f>
@@ -1110,10 +1098,10 @@
     <row r="23" spans="1:4" ht="53.25" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="20">
         <v>24</v>
@@ -1122,10 +1110,10 @@
     <row r="24" spans="1:4" ht="53.25" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" s="20">
         <v>24</v>
@@ -1134,10 +1122,10 @@
     <row r="25" spans="1:4" ht="53.25" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="25">
         <v>48</v>
@@ -1152,10 +1140,10 @@
     <row r="27" spans="1:4" ht="27.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="11">
         <f>SUM(D28:D30)</f>
@@ -1165,10 +1153,10 @@
     <row r="28" spans="1:4" ht="43.5" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28" s="20">
         <v>24</v>
@@ -1177,10 +1165,10 @@
     <row r="29" spans="1:4" ht="43.5" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="30">
         <v>24</v>
@@ -1189,10 +1177,10 @@
     <row r="30" spans="1:4" ht="43.5" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="25">
         <v>4</v>
@@ -1207,10 +1195,10 @@
     <row r="32" spans="1:4" ht="27.75" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="11">
         <f>SUM(D33:D35)</f>
@@ -1220,10 +1208,10 @@
     <row r="33" spans="1:4" ht="30.75" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="20">
         <v>15</v>
@@ -1232,10 +1220,10 @@
     <row r="34" spans="1:4" ht="30.75" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="20">
         <v>15</v>
@@ -1244,10 +1232,10 @@
     <row r="35" spans="1:4" ht="30.75" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D35" s="25">
         <v>15</v>

</xml_diff>